<commit_message>
02Feb2022 Selenium DataDriven Part2"
</commit_message>
<xml_diff>
--- a/src/test/resources/AutomationDemoSIte.xlsx
+++ b/src/test/resources/AutomationDemoSIte.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspaces\DecSelenium2021_8_00AM_IST\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{384360CF-A366-421D-821A-5BBA59353F10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF0DB63D-0C92-4419-961F-E5A9E7A3D83E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{9F696F77-14B2-4A68-A1B1-E5EA60DF3651}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="97">
   <si>
     <t>RunMode</t>
   </si>
@@ -327,6 +327,9 @@
   </si>
   <si>
     <t>validateDataDriven</t>
+  </si>
+  <si>
+    <t>Cricket &amp; Hockey</t>
   </si>
 </sst>
 </file>
@@ -714,8 +717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88A98684-4136-4155-A927-F35C3B12F23B}">
   <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2:S6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -724,6 +727,7 @@
     <col min="2" max="2" width="15.9296875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="12.59765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.1328125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.33203125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="13" max="13" width="16.86328125" customWidth="1" collapsed="1"/>
     <col min="18" max="18" width="15.33203125" bestFit="1" customWidth="1" collapsed="1"/>
@@ -814,7 +818,7 @@
         <v>44</v>
       </c>
       <c r="I2" t="s">
-        <v>47</v>
+        <v>96</v>
       </c>
       <c r="J2" t="s">
         <v>50</v>

</xml_diff>

<commit_message>
03Feb2022 Selenium DataDriven Part3
</commit_message>
<xml_diff>
--- a/src/test/resources/AutomationDemoSIte.xlsx
+++ b/src/test/resources/AutomationDemoSIte.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspaces\DecSelenium2021_8_00AM_IST\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF0DB63D-0C92-4419-961F-E5A9E7A3D83E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{150E392D-8FE5-4E6D-82F5-594DBDEE0A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{9F696F77-14B2-4A68-A1B1-E5EA60DF3651}"/>
   </bookViews>
@@ -329,7 +329,7 @@
     <t>validateDataDriven</t>
   </si>
   <si>
-    <t>Cricket &amp; Hockey</t>
+    <t>Cricket&amp;Hockey</t>
   </si>
 </sst>
 </file>
@@ -718,7 +718,7 @@
   <dimension ref="A1:S8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
04Feb2022 Selenium DataDriven Part4
</commit_message>
<xml_diff>
--- a/src/test/resources/AutomationDemoSIte.xlsx
+++ b/src/test/resources/AutomationDemoSIte.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspaces\DecSelenium2021_8_00AM_IST\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{150E392D-8FE5-4E6D-82F5-594DBDEE0A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3550728-F8DA-425D-BC15-C6C3490447AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{9F696F77-14B2-4A68-A1B1-E5EA60DF3651}"/>
   </bookViews>
@@ -263,9 +263,6 @@
     <t>Japan</t>
   </si>
   <si>
-    <t>Netherlanda</t>
-  </si>
-  <si>
     <t>South Africa</t>
   </si>
   <si>
@@ -330,6 +327,9 @@
   </si>
   <si>
     <t>Cricket&amp;Hockey</t>
+  </si>
+  <si>
+    <t>Netherlands</t>
   </si>
 </sst>
 </file>
@@ -718,7 +718,7 @@
   <dimension ref="A1:S8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -738,7 +738,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -789,15 +789,15 @@
         <v>15</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
@@ -818,7 +818,7 @@
         <v>44</v>
       </c>
       <c r="I2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J2" t="s">
         <v>50</v>
@@ -836,25 +836,25 @@
         <v>1987</v>
       </c>
       <c r="O2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="P2">
         <v>5</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="S2" s="8"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C3" t="s">
         <v>45</v>
@@ -893,25 +893,25 @@
         <v>1988</v>
       </c>
       <c r="O3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="P3">
         <v>9</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S3" s="9"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C4" t="s">
         <v>18</v>
@@ -950,25 +950,25 @@
         <v>1989</v>
       </c>
       <c r="O4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="P4">
         <v>14</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="S4" s="3"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C5" t="s">
         <v>19</v>
@@ -1007,25 +1007,25 @@
         <v>1990</v>
       </c>
       <c r="O5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="P5">
         <v>18</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="S5" s="10"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C6" t="s">
         <v>20</v>
@@ -1058,31 +1058,31 @@
         <v>68</v>
       </c>
       <c r="M6" t="s">
-        <v>74</v>
+        <v>96</v>
       </c>
       <c r="N6">
         <v>1991</v>
       </c>
       <c r="O6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P6">
         <v>21</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="S6" s="6"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C7" t="s">
         <v>21</v>
@@ -1115,31 +1115,31 @@
         <v>69</v>
       </c>
       <c r="M7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="N7">
         <v>1992</v>
       </c>
       <c r="O7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P7">
         <v>27</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="S7" s="4"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C8" t="s">
         <v>22</v>
@@ -1172,22 +1172,22 @@
         <v>70</v>
       </c>
       <c r="M8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="N8">
         <v>1993</v>
       </c>
       <c r="O8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P8">
         <v>30</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="S8" s="7"/>
     </row>

</xml_diff>